<commit_message>
Actualización de mi setup
</commit_message>
<xml_diff>
--- a/Radiation.xlsx
+++ b/Radiation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\nabernal10\OpenFOAM\windTunnel_Tree\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{415B8F4A-AE47-4D9D-BD6D-3ABF0D26706F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9F10A45-563F-43EE-BC7E-1D018D2F90C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{4466A985-D6EE-441A-8DEC-8066E2B76AAD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{4466A985-D6EE-441A-8DEC-8066E2B76AAD}"/>
   </bookViews>
   <sheets>
     <sheet name="Case set up" sheetId="2" r:id="rId1"/>
@@ -1026,12 +1026,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1039,6 +1033,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4853,19 +4853,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>8.888888888888431</c:v>
+                  <c:v>8.7777777777773256</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>8.888888888888431</c:v>
+                  <c:v>8.7777777777773256</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>8.888888888888431</c:v>
+                  <c:v>8.7777777777773256</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>8.888888888888431</c:v>
+                  <c:v>8.7777777777773256</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>8.888888888888431</c:v>
+                  <c:v>8.7777777777773256</c:v>
                 </c:pt>
                 <c:pt idx="105">
                   <c:v>0</c:v>
@@ -5949,16 +5949,16 @@
                   <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>81.778039273339431</c:v>
+                  <c:v>81.973631453690857</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>67.551997044362082</c:v>
+                  <c:v>67.875517714197329</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>55.800705730165163</c:v>
+                  <c:v>56.202047210425029</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>46.093659643247513</c:v>
+                  <c:v>46.536221262326436</c:v>
                 </c:pt>
                 <c:pt idx="105">
                   <c:v>99</c:v>
@@ -24597,9 +24597,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC8191BD-2B7B-4602-AB98-101ED92BF2DD}">
   <dimension ref="B2:Q116"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
+      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -25013,13 +25013,13 @@
       <c r="D10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="30">
+      <c r="E10" s="28">
         <v>0.215</v>
       </c>
-      <c r="F10" s="31">
+      <c r="F10" s="29">
         <v>0.78</v>
       </c>
-      <c r="G10" s="31">
+      <c r="G10" s="29">
         <f>F10-E10</f>
         <v>0.56500000000000006</v>
       </c>
@@ -25072,7 +25072,7 @@
       </c>
       <c r="E11" s="5">
         <f>E12/(E8-E9)</f>
-        <v>8.888888888888431</v>
+        <v>8.7777777777773256</v>
       </c>
       <c r="F11" s="4">
         <v>8.77</v>
@@ -25125,7 +25125,7 @@
         <v>19</v>
       </c>
       <c r="E12" s="2">
-        <v>4</v>
+        <v>3.95</v>
       </c>
       <c r="H12" s="2">
         <f t="shared" si="1"/>
@@ -25278,7 +25278,7 @@
       </c>
       <c r="E15" s="2">
         <f>SUM(P3:P116)/E11</f>
-        <v>59.519632901349567</v>
+        <v>59.768861853048875</v>
       </c>
       <c r="H15" s="2">
         <f t="shared" si="1"/>
@@ -28642,7 +28642,7 @@
       </c>
       <c r="L103" s="2">
         <f t="shared" si="16"/>
-        <v>8.888888888888431</v>
+        <v>8.7777777777773256</v>
       </c>
       <c r="M103" s="2">
         <f t="shared" si="17"/>
@@ -28680,7 +28680,7 @@
       </c>
       <c r="L104" s="2">
         <f t="shared" si="16"/>
-        <v>8.888888888888431</v>
+        <v>8.7777777777773256</v>
       </c>
       <c r="M104" s="2">
         <f t="shared" si="17"/>
@@ -28688,19 +28688,19 @@
       </c>
       <c r="N104" s="2">
         <f t="shared" si="23"/>
-        <v>0.82604080074080233</v>
+        <v>0.82801647933021072</v>
       </c>
       <c r="O104" s="2">
         <f>N104*$E$4</f>
-        <v>81.778039273339431</v>
+        <v>81.973631453690857</v>
       </c>
       <c r="P104" s="2">
         <f>(O103-O104)/J104*M104</f>
-        <v>172.21960726660555</v>
+        <v>170.26368546309129</v>
       </c>
       <c r="Q104" s="4">
         <f>P104/$E$11</f>
-        <v>19.374705817494121</v>
+        <v>19.397128723644311</v>
       </c>
     </row>
     <row r="105" spans="8:17" x14ac:dyDescent="0.3">
@@ -28722,7 +28722,7 @@
       </c>
       <c r="L105" s="2">
         <f t="shared" si="16"/>
-        <v>8.888888888888431</v>
+        <v>8.7777777777773256</v>
       </c>
       <c r="M105" s="2">
         <f t="shared" si="17"/>
@@ -28730,19 +28730,19 @@
       </c>
       <c r="N105" s="2">
         <f t="shared" si="23"/>
-        <v>0.68234340448850583</v>
+        <v>0.68561129004239729</v>
       </c>
       <c r="O105" s="2">
         <f t="shared" ref="O105:O113" si="25">N105*$E$4</f>
-        <v>67.551997044362082</v>
+        <v>67.875517714197329</v>
       </c>
       <c r="P105" s="2">
         <f t="shared" si="20"/>
-        <v>142.26042228977337</v>
+        <v>140.98113739493516</v>
       </c>
       <c r="Q105" s="4">
         <f t="shared" ref="Q105:Q107" si="26">P105/$E$11</f>
-        <v>16.004297507600327</v>
+        <v>16.061142234866857</v>
       </c>
     </row>
     <row r="106" spans="8:17" x14ac:dyDescent="0.3">
@@ -28764,7 +28764,7 @@
       </c>
       <c r="L106" s="2">
         <f t="shared" si="16"/>
-        <v>8.888888888888431</v>
+        <v>8.7777777777773256</v>
       </c>
       <c r="M106" s="2">
         <f t="shared" si="17"/>
@@ -28772,19 +28772,19 @@
       </c>
       <c r="N106" s="2">
         <f t="shared" si="23"/>
-        <v>0.56364349222389054</v>
+        <v>0.5676974465699498</v>
       </c>
       <c r="O106" s="2">
         <f t="shared" si="25"/>
-        <v>55.800705730165163</v>
+        <v>56.202047210425029</v>
       </c>
       <c r="P106" s="2">
         <f t="shared" si="20"/>
-        <v>117.51291314196909</v>
+        <v>116.7347050377229</v>
       </c>
       <c r="Q106" s="4">
         <f t="shared" si="26"/>
-        <v>13.220202728472204</v>
+        <v>13.298890447336206</v>
       </c>
     </row>
     <row r="107" spans="8:17" x14ac:dyDescent="0.3">
@@ -28806,7 +28806,7 @@
       </c>
       <c r="L107" s="2">
         <f t="shared" si="16"/>
-        <v>8.888888888888431</v>
+        <v>8.7777777777773256</v>
       </c>
       <c r="M107" s="2">
         <f t="shared" si="17"/>
@@ -28814,19 +28814,19 @@
       </c>
       <c r="N107" s="2">
         <f t="shared" si="23"/>
-        <v>0.46559252164896475</v>
+        <v>0.47006284103360035</v>
       </c>
       <c r="O107" s="2">
         <f>N107*$E$4</f>
-        <v>46.093659643247513</v>
+        <v>46.536221262326436</v>
       </c>
       <c r="P107" s="2">
         <f t="shared" si="20"/>
-        <v>97.070460869176529</v>
+        <v>96.658259480985961</v>
       </c>
       <c r="Q107" s="4">
         <f t="shared" si="26"/>
-        <v>10.920426847782922</v>
+        <v>11.0117004472015</v>
       </c>
     </row>
     <row r="108" spans="8:17" x14ac:dyDescent="0.3">
@@ -29186,7 +29186,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCA11A4A-1940-4341-A6C9-DCAF48DA6B48}">
   <dimension ref="B2:L123"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
     </sheetView>
@@ -30912,7 +30912,7 @@
       </c>
     </row>
     <row r="91" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B91" s="29">
+      <c r="B91" s="27">
         <f>E91/D88</f>
         <v>45.964285714285715</v>
       </c>
@@ -32545,13 +32545,13 @@
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
       <c r="J7" s="12"/>
-      <c r="K7" s="28" t="s">
+      <c r="K7" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="L7" s="27" t="s">
+      <c r="L7" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="M7" s="27"/>
+      <c r="M7" s="30"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="23" t="s">
@@ -32576,7 +32576,7 @@
       <c r="J8" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="K8" s="28"/>
+      <c r="K8" s="31"/>
       <c r="L8" s="26" t="s">
         <v>98</v>
       </c>

</xml_diff>